<commit_message>
add: FFmeter improved, almost finished
</commit_message>
<xml_diff>
--- a/control_software/Filter function meter/Template/Example of FF meter template.xlsx
+++ b/control_software/Filter function meter/Template/Example of FF meter template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\martin\WAC\WACsw - github\control_software\Filter function meter\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED17114A-0925-408D-909C-78F85E7358D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE9A72D-2A47-447B-ACDD-AD1F1935D6A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="14775" xr2:uid="{B3798027-E95D-4306-B018-FE372260F1B7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{B3798027-E95D-4306-B018-FE372260F1B7}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -418,7 +418,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -1452,7 +1452,7 @@
   <dimension ref="A1:AI116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1726,6 +1726,7 @@
       <c r="O13" s="11"/>
       <c r="P13" s="11"/>
       <c r="Q13" s="11"/>
+      <c r="R13" s="11"/>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B14" s="8">

</xml_diff>

<commit_message>
fix: FFmeter: button colors on hover
</commit_message>
<xml_diff>
--- a/control_software/Filter function meter/Template/Example of FF meter template.xlsx
+++ b/control_software/Filter function meter/Template/Example of FF meter template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\martin\WAC\WACsw - github\control_software\Filter function meter\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDB5A1DE-A3D3-4BB1-BA9E-E598082EDADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9EDFD76-41FF-4C52-BBCB-04AD7EFD1EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23970" windowHeight="14370" xr2:uid="{B3798027-E95D-4306-B018-FE372260F1B7}"/>
+    <workbookView xWindow="2685" yWindow="2235" windowWidth="17805" windowHeight="10290" xr2:uid="{B3798027-E95D-4306-B018-FE372260F1B7}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
   <si>
     <t>Signal frequency</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>HP3458A</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -5315,16 +5318,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>92448</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>94970</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>397248</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>142595</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>344579</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>171170</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>649379</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>28295</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5652,7 +5655,7 @@
   <dimension ref="A1:AJ1999"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H21" sqref="D10:H21"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5846,48 +5849,58 @@
         <f>B10</f>
         <v>10000</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
+      <c r="D10" s="8">
+        <v>45638.867291666669</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="12">
+        <v>-1.693694603443</v>
+      </c>
+      <c r="H10" s="12">
+        <v>1.2244894232060001E-4</v>
+      </c>
       <c r="I10" s="18">
         <f>IF(ISEVEN(ROW()),B10/1000,"")</f>
         <v>10</v>
       </c>
       <c r="J10" s="17" t="e">
         <f>IF(B10&gt;B11,E10*G10/G11,NA())</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="K10" s="12">
-        <v>-6.4576916396619999E-2</v>
+        <v>-1.693062782288</v>
       </c>
       <c r="L10" s="12">
-        <v>-6.1558388173580003E-2</v>
+        <v>-1.693238139153</v>
       </c>
       <c r="M10" s="12">
-        <v>-6.1362534761429999E-2</v>
+        <v>-1.693436026573</v>
       </c>
       <c r="N10" s="12">
-        <v>-5.9963483363389997E-2</v>
+        <v>-1.6935094594960001</v>
       </c>
       <c r="O10" s="12">
-        <v>-5.7080112397670003E-2</v>
+        <v>-1.693641781807</v>
       </c>
       <c r="P10" s="12">
-        <v>-4.8210076987739998E-2</v>
+        <v>-1.693772554398</v>
       </c>
       <c r="Q10" s="9">
-        <v>-4.4330731034280001E-2</v>
+        <v>-1.6938751935959999</v>
       </c>
       <c r="R10" s="11">
-        <v>-3.3033009618520001E-2</v>
+        <v>-1.6940512657169999</v>
       </c>
       <c r="S10" s="12">
-        <v>-2.256765216589E-2</v>
+        <v>-1.6941480636599999</v>
       </c>
       <c r="T10" s="12">
-        <v>-2.3786555975679999E-2</v>
+        <v>-1.6942107677460001</v>
       </c>
       <c r="U10" s="12"/>
       <c r="V10" s="12"/>
@@ -5915,11 +5928,21 @@
         <f t="shared" ref="C11:C74" si="0">B11</f>
         <v>1000</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
+      <c r="D11" s="8">
+        <v>45638.867731481485</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="12">
+        <v>-1.6942984342580001</v>
+      </c>
+      <c r="H11" s="12">
+        <v>4.3287051619019999E-5</v>
+      </c>
       <c r="I11" s="18" t="str">
         <f t="shared" ref="I11:I12" si="1">IF(ISEVEN(ROW()),B11/1000,"")</f>
         <v/>
@@ -5929,34 +5952,34 @@
         <v>#N/A</v>
       </c>
       <c r="K11" s="12">
-        <v>-1.8481750041250002E-2</v>
+        <v>-1.694246888161</v>
       </c>
       <c r="L11" s="12">
-        <v>8.0376183614130001E-3</v>
+        <v>-1.6942647695540001</v>
       </c>
       <c r="M11" s="12">
-        <v>-2.0281689241529999E-2</v>
+        <v>-1.6942031383509999</v>
       </c>
       <c r="N11" s="12">
-        <v>-3.5037476569410003E-2</v>
+        <v>-1.694157958031</v>
       </c>
       <c r="O11" s="12">
-        <v>-5.3610943257809997E-2</v>
+        <v>-1.69415640831</v>
       </c>
       <c r="P11" s="12">
-        <v>-7.2013750672340004E-2</v>
+        <v>-1.6942203044890001</v>
       </c>
       <c r="Q11" s="12">
-        <v>-7.8909918665890005E-2</v>
+        <v>-1.6943058967589999</v>
       </c>
       <c r="R11" s="11">
-        <v>-7.8457526862620003E-2</v>
+        <v>-1.694393515587</v>
       </c>
       <c r="S11" s="12">
-        <v>-6.4419031143190003E-2</v>
+        <v>-1.6944704055790001</v>
       </c>
       <c r="T11" s="12">
-        <v>-5.6967325508590003E-2</v>
+        <v>-1.694565057755</v>
       </c>
       <c r="U11" s="12"/>
       <c r="V11" s="12"/>
@@ -5984,48 +6007,58 @@
         <f t="shared" si="0"/>
         <v>20000</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
+      <c r="D12" s="8">
+        <v>45638.868159722224</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" s="12">
+        <v>-1.694568181038</v>
+      </c>
+      <c r="H12" s="12">
+        <v>2.4037977087259999E-5</v>
+      </c>
       <c r="I12" s="18">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="J12" s="17" t="e">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="K12" s="12">
-        <v>-5.204832553864E-2</v>
+        <v>-1.6946179866790001</v>
       </c>
       <c r="L12" s="12">
-        <v>-5.44750019908E-2</v>
+        <v>-1.69462120533</v>
       </c>
       <c r="M12" s="12">
-        <v>-5.6231345981360002E-2</v>
+        <v>-1.6945910453799999</v>
       </c>
       <c r="N12" s="12">
-        <v>-5.4909761995079999E-2</v>
+        <v>-1.6945368051530001</v>
       </c>
       <c r="O12" s="12">
-        <v>-5.3857233375310003E-2</v>
+        <v>-1.694498181343</v>
       </c>
       <c r="P12" s="12">
-        <v>-5.0292439758779998E-2</v>
+        <v>-1.694471716881</v>
       </c>
       <c r="Q12" s="12">
-        <v>-4.5585300773380001E-2</v>
+        <v>-1.694502472878</v>
       </c>
       <c r="R12" s="11">
-        <v>-4.1622564196590002E-2</v>
+        <v>-1.6945098638530001</v>
       </c>
       <c r="S12" s="12">
-        <v>-2.7572656050319999E-2</v>
+        <v>-1.6946213245390001</v>
       </c>
       <c r="T12" s="12">
-        <v>-3.0835200101139999E-2</v>
+        <v>-1.6947112083439999</v>
       </c>
       <c r="U12" s="12"/>
       <c r="V12" s="12"/>
@@ -6045,11 +6078,21 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
+      <c r="D13" s="8">
+        <v>45638.868414351855</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="12">
+        <v>-1.6948587894439999</v>
+      </c>
+      <c r="H13" s="12">
+        <v>2.701218669661E-5</v>
+      </c>
       <c r="I13" s="18" t="str">
         <f t="shared" ref="I13:I76" si="3">IF(ISEVEN(ROW()),B13/1000,"")</f>
         <v/>
@@ -6059,34 +6102,34 @@
         <v>#N/A</v>
       </c>
       <c r="K13" s="12">
-        <v>-3.8672883063549997E-2</v>
+        <v>-1.6948082447049999</v>
       </c>
       <c r="L13" s="12">
-        <v>-4.039815813303E-2</v>
+        <v>-1.694924592972</v>
       </c>
       <c r="M13" s="12">
-        <v>-3.6857448518280003E-2</v>
+        <v>-1.6949737071990001</v>
       </c>
       <c r="N13" s="12">
-        <v>-3.5085290670389999E-2</v>
+        <v>-1.694981813431</v>
       </c>
       <c r="O13" s="12">
-        <v>-3.275098651648E-2</v>
+        <v>-1.6948471069340001</v>
       </c>
       <c r="P13" s="12">
-        <v>-3.3421199768779997E-2</v>
+        <v>-1.6948418617250001</v>
       </c>
       <c r="Q13" s="12">
-        <v>-3.3962815999980002E-2</v>
+        <v>-1.6947444677350001</v>
       </c>
       <c r="R13" s="11">
-        <v>-3.89613173902E-2</v>
+        <v>-1.694740772247</v>
       </c>
       <c r="S13" s="12">
-        <v>-5.9888578951360003E-2</v>
+        <v>-1.6948239803309999</v>
       </c>
       <c r="T13" s="12">
-        <v>-5.6298218667510003E-2</v>
+        <v>-1.6949013471600001</v>
       </c>
       <c r="U13" s="12"/>
       <c r="V13" s="12"/>
@@ -6106,48 +6149,58 @@
         <f t="shared" si="0"/>
         <v>30000</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
+      <c r="D14" s="8">
+        <v>45638.868842592594</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" s="12">
+        <v>-1.6951008915900001</v>
+      </c>
+      <c r="H14" s="12">
+        <v>1.787841251039E-5</v>
+      </c>
       <c r="I14" s="18">
         <f t="shared" si="3"/>
         <v>30</v>
       </c>
       <c r="J14" s="17" t="e">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="K14" s="12">
-        <v>-5.8567371219399998E-2</v>
+        <v>-1.695010781288</v>
       </c>
       <c r="L14" s="12">
-        <v>-6.043149530888E-2</v>
+        <v>-1.6951072216030001</v>
       </c>
       <c r="M14" s="12">
-        <v>-5.3964227437969997E-2</v>
+        <v>-1.695170283318</v>
       </c>
       <c r="N14" s="12">
-        <v>-4.6396840363739998E-2</v>
+        <v>-1.6951602697370001</v>
       </c>
       <c r="O14" s="12">
-        <v>-4.2893495410680001E-2</v>
+        <v>-1.6951638460159999</v>
       </c>
       <c r="P14" s="12">
-        <v>-3.6631189286709998E-2</v>
+        <v>-1.695112705231</v>
       </c>
       <c r="Q14" s="12">
-        <v>-3.4129176288839998E-2</v>
+        <v>-1.6950497627259999</v>
       </c>
       <c r="R14" s="11">
-        <v>-3.077773377299E-2</v>
+        <v>-1.695036053658</v>
       </c>
       <c r="S14" s="12">
-        <v>-5.7101260870699999E-2</v>
+        <v>-1.6950731277469999</v>
       </c>
       <c r="T14" s="12">
-        <v>-4.7766823321579999E-2</v>
+        <v>-1.6951248645779999</v>
       </c>
       <c r="U14" s="12"/>
       <c r="V14" s="12"/>
@@ -6167,11 +6220,21 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
+      <c r="D15" s="8">
+        <v>45638.869270833333</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="12">
+        <v>-1.695297598839</v>
+      </c>
+      <c r="H15" s="12">
+        <v>2.7030564385130001E-5</v>
+      </c>
       <c r="I15" s="18" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -6181,34 +6244,34 @@
         <v>#N/A</v>
       </c>
       <c r="K15" s="12">
-        <v>-4.3327562510970002E-2</v>
+        <v>-1.695212006569</v>
       </c>
       <c r="L15" s="12">
-        <v>-4.207770898938E-2</v>
+        <v>-1.6953321695329999</v>
       </c>
       <c r="M15" s="12">
-        <v>-4.4634431600569999E-2</v>
+        <v>-1.6954143047329999</v>
       </c>
       <c r="N15" s="12">
-        <v>-4.6940267086030003E-2</v>
+        <v>-1.69541478157</v>
       </c>
       <c r="O15" s="12">
-        <v>-4.9305357038970002E-2</v>
+        <v>-1.69536626339</v>
       </c>
       <c r="P15" s="12">
-        <v>-5.1706481724979998E-2</v>
+        <v>-1.6953303813930001</v>
       </c>
       <c r="Q15" s="12">
-        <v>-5.2684154361490002E-2</v>
+        <v>-1.6952613592150001</v>
       </c>
       <c r="R15" s="11">
-        <v>-5.3688354790210002E-2</v>
+        <v>-1.695180892944</v>
       </c>
       <c r="S15" s="12">
-        <v>-5.616617947817E-2</v>
+        <v>-1.695215582848</v>
       </c>
       <c r="T15" s="12">
-        <v>-5.1934126764539998E-2</v>
+        <v>-1.6952482461930001</v>
       </c>
       <c r="U15" s="12"/>
       <c r="V15" s="12"/>
@@ -6228,48 +6291,58 @@
         <f t="shared" si="0"/>
         <v>40000</v>
       </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
+      <c r="D16" s="8">
+        <v>45638.869710648149</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="12">
+        <v>-1.6955108761790001</v>
+      </c>
+      <c r="H16" s="12">
+        <v>3.104198327892E-5</v>
+      </c>
       <c r="I16" s="18">
         <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="J16" s="17" t="e">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="K16" s="12">
-        <v>-4.595948010683E-2</v>
+        <v>-1.695322871208</v>
       </c>
       <c r="L16" s="12">
-        <v>-4.6821270138030002E-2</v>
+        <v>-1.695373415947</v>
       </c>
       <c r="M16" s="12">
-        <v>-4.7730762511489999E-2</v>
+        <v>-1.695498108864</v>
       </c>
       <c r="N16" s="12">
-        <v>-5.1110286265609997E-2</v>
+        <v>-1.6955516338350001</v>
       </c>
       <c r="O16" s="12">
-        <v>-5.0676818937059998E-2</v>
+        <v>-1.6956192255019999</v>
       </c>
       <c r="P16" s="12">
-        <v>-5.0806939601899997E-2</v>
+        <v>-1.695605516434</v>
       </c>
       <c r="Q16" s="12">
-        <v>-5.0886325538159999E-2</v>
+        <v>-1.6956051588059999</v>
       </c>
       <c r="R16" s="11">
-        <v>-4.49976362288E-2</v>
+        <v>-1.6955375671390001</v>
       </c>
       <c r="S16" s="12">
-        <v>-5.512585490942E-2</v>
+        <v>-1.6954953670499999</v>
       </c>
       <c r="T16" s="12">
-        <v>-5.2927803248170001E-2</v>
+        <v>-1.695499897003</v>
       </c>
       <c r="U16" s="12"/>
       <c r="V16" s="12"/>

</xml_diff>